<commit_message>
Updated DB with data
</commit_message>
<xml_diff>
--- a/SAD Sampl Data.xlsx
+++ b/SAD Sampl Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akaybanez\Documents\GitHub\FinalSoftEngRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3F70A109-1E94-4335-8365-BF66B2D341AC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="11055" xr2:uid="{492F95E8-F61A-4328-81A4-066721DC7F7F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -346,7 +345,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,12 +390,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -412,7 +417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -423,20 +428,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -751,11 +773,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E2EEB3-701C-4AAD-A3D8-BD3C5B797E51}">
-  <dimension ref="A1:I63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +786,7 @@
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="24.7109375" customWidth="1"/>
@@ -784,216 +806,216 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:9" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="10">
         <v>35877</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:9" s="8" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="10">
         <v>35878</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:9" s="8" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="10">
         <v>35879</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:9" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="10">
         <v>35880</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="1:9" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="10">
         <v>35881</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="10">
         <v>35882</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="14">
         <v>35883</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+    <row r="14" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1003,303 +1025,303 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>51</v>
+    <row r="21" spans="2:3" ht="36" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>53</v>
+      <c r="B22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>54</v>
+      <c r="B24" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>55</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" ht="36" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
-        <v>71</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="43" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C43" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D43" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E46">
+      <c r="E43" s="8">
         <v>552015556</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="44" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C44" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D44" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E47">
+      <c r="E44" s="8">
         <v>552015556</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="45" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C45" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D45" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E48">
+      <c r="E45" s="8">
         <v>552015556</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="46" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C46" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D46" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E49">
+      <c r="E46" s="8">
         <v>552015556</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="47" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C47" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D47" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E50">
+      <c r="E47" s="8">
         <v>552015556</v>
       </c>
     </row>
+    <row r="48" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E48" s="8">
+        <v>552015556</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="9">
+        <v>552015556</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" s="8">
+        <v>552015556</v>
+      </c>
+    </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>68</v>
+      <c r="B51" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="C51" t="s">
         <v>74</v>
       </c>
       <c r="D51" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E51">
         <v>552015556</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" t="s">
-        <v>74</v>
-      </c>
-      <c r="D52" t="s">
-        <v>77</v>
-      </c>
-      <c r="E52">
-        <v>552015556</v>
-      </c>
-    </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>70</v>
-      </c>
-      <c r="C53" t="s">
-        <v>74</v>
-      </c>
-      <c r="D53" t="s">
-        <v>80</v>
-      </c>
-      <c r="E53">
-        <v>552015556</v>
+      <c r="A53" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C54" t="s">
-        <v>74</v>
-      </c>
-      <c r="D54" t="s">
-        <v>81</v>
-      </c>
-      <c r="E54">
-        <v>552015556</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>90</v>
+      <c r="B54" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>91</v>
+      <c r="B57" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B58" s="3" t="s">
-        <v>92</v>
+      <c r="B58" s="6" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B63" s="3" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{6FCEC935-2710-4404-8A25-13FFB07D2582}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{C203F04B-325C-4FF5-B039-E6BAD44B3913}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{4E9BCCE8-D702-4D10-9C94-3BE011B663F1}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{80250314-9609-4F0C-A961-42DB5175667A}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{7B7FC64C-F918-4E77-973F-B7511BDB0865}"/>
-    <hyperlink ref="I7" r:id="rId6" xr:uid="{B3F6C826-1BEA-4E70-BB75-19E72ECE4321}"/>
-    <hyperlink ref="I8" r:id="rId7" xr:uid="{FB118608-32A6-41E0-A4A9-64A1A0D5717D}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId8"/>

</xml_diff>